<commit_message>
Tweaks to allow for no timelines and a test file
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/minimum.xlsx
+++ b/tests/integration_test_files/minimum.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/github/usdm_data/source_data/training/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/github/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7219E92-AB5A-F741-8AAE-65B7A9BA1714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7F217B-874E-FF45-BF81-40DED33CEE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="660" windowWidth="36420" windowHeight="17380" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="820" yWindow="660" windowWidth="36420" windowHeight="17380" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -21,31 +21,29 @@
     <sheet name="studyDesignEligibilityCriteria" sheetId="5" r:id="rId6"/>
     <sheet name="studyDesignArms" sheetId="6" r:id="rId7"/>
     <sheet name="studyDesignEpochs" sheetId="7" r:id="rId8"/>
-    <sheet name="mainTimeline" sheetId="8" r:id="rId9"/>
-    <sheet name="studyDesignTiming" sheetId="12" r:id="rId10"/>
-    <sheet name="studyDesignActivities" sheetId="13" r:id="rId11"/>
-    <sheet name="studyDesignInterventions" sheetId="14" r:id="rId12"/>
-    <sheet name="studyDesignIndications" sheetId="15" r:id="rId13"/>
-    <sheet name="studyDesignPopulations" sheetId="16" r:id="rId14"/>
-    <sheet name="studyDesignCharacteristics" sheetId="17" r:id="rId15"/>
-    <sheet name="studyDesignOE" sheetId="18" r:id="rId16"/>
-    <sheet name="studyDesignEstimands" sheetId="19" r:id="rId17"/>
-    <sheet name="studyDesignProcedures" sheetId="20" r:id="rId18"/>
-    <sheet name="studyDesignEncounters" sheetId="21" r:id="rId19"/>
-    <sheet name="studyDesignElements" sheetId="22" r:id="rId20"/>
-    <sheet name="dictionaries" sheetId="23" r:id="rId21"/>
-    <sheet name="documentContent" sheetId="27" r:id="rId22"/>
-    <sheet name="people" sheetId="30" r:id="rId23"/>
-    <sheet name="roles" sheetId="29" r:id="rId24"/>
-    <sheet name="studyDesignSites" sheetId="31" r:id="rId25"/>
-    <sheet name="configuration" sheetId="26" r:id="rId26"/>
+    <sheet name="studyDesignActivities" sheetId="13" r:id="rId9"/>
+    <sheet name="studyDesignInterventions" sheetId="14" r:id="rId10"/>
+    <sheet name="studyDesignIndications" sheetId="15" r:id="rId11"/>
+    <sheet name="studyDesignPopulations" sheetId="16" r:id="rId12"/>
+    <sheet name="studyDesignCharacteristics" sheetId="17" r:id="rId13"/>
+    <sheet name="studyDesignOE" sheetId="18" r:id="rId14"/>
+    <sheet name="studyDesignEstimands" sheetId="19" r:id="rId15"/>
+    <sheet name="studyDesignProcedures" sheetId="20" r:id="rId16"/>
+    <sheet name="studyDesignEncounters" sheetId="21" r:id="rId17"/>
+    <sheet name="studyDesignElements" sheetId="22" r:id="rId18"/>
+    <sheet name="dictionaries" sheetId="23" r:id="rId19"/>
+    <sheet name="documentContent" sheetId="27" r:id="rId20"/>
+    <sheet name="people" sheetId="30" r:id="rId21"/>
+    <sheet name="roles" sheetId="29" r:id="rId22"/>
+    <sheet name="studyDesignSites" sheetId="31" r:id="rId23"/>
+    <sheet name="configuration" sheetId="26" r:id="rId24"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="181">
   <si>
     <t>name</t>
   </si>
@@ -266,90 +264,12 @@
     <t>SCREENING</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Main Timeline</t>
-  </si>
-  <si>
-    <t>DOSE</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>This is the main timeline for the study design.</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Condition</t>
-  </si>
-  <si>
-    <t>Potential subject identified</t>
-  </si>
-  <si>
-    <t>Activity</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>(EXIT)</t>
-  </si>
-  <si>
-    <t>condition</t>
-  </si>
-  <si>
-    <t>epoch</t>
-  </si>
-  <si>
-    <t>encounter</t>
-  </si>
-  <si>
     <t>E1</t>
   </si>
   <si>
-    <t>Parent Activity</t>
-  </si>
-  <si>
-    <t>Child Activity</t>
-  </si>
-  <si>
-    <t>BC/Procedure/Timeline</t>
-  </si>
-  <si>
     <t>Informed consent</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>from</t>
-  </si>
-  <si>
-    <t>to</t>
-  </si>
-  <si>
-    <t>timingValue</t>
-  </si>
-  <si>
-    <t>toFrom</t>
-  </si>
-  <si>
-    <t>window</t>
-  </si>
-  <si>
-    <t>TIM1</t>
-  </si>
-  <si>
-    <t>FIXED</t>
-  </si>
-  <si>
-    <t>1 Day</t>
-  </si>
-  <si>
     <t>activityIsConditional</t>
   </si>
   <si>
@@ -624,15 +544,6 @@
   </si>
   <si>
     <t>The Arm</t>
-  </si>
-  <si>
-    <t>Anchor</t>
-  </si>
-  <si>
-    <t>The anchor</t>
-  </si>
-  <si>
-    <t>The Only One</t>
   </si>
   <si>
     <t>BOTH</t>
@@ -757,22 +668,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1201,163 +1103,163 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
+      <c r="B2" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="B3" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="30">
+      <c r="B4" s="27">
         <v>1</v>
       </c>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>199</v>
-      </c>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
+      <c r="B5" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
     </row>
     <row r="6" spans="1:7" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
+      <c r="B6" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
     </row>
     <row r="7" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
+      <c r="B7" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
+      <c r="B8" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
     </row>
     <row r="9" spans="1:7" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
+      <c r="B9" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
     </row>
     <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
+      <c r="B10" s="10"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
+      <c r="B11" s="10"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="30">
+      <c r="B12" s="27">
         <v>1</v>
       </c>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="32" t="s">
+      <c r="D15" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="32" t="s">
+      <c r="G15" s="29" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C16" t="s">
@@ -1369,7 +1271,7 @@
       <c r="E16" t="s">
         <v>27</v>
       </c>
-      <c r="F16" s="33">
+      <c r="F16" s="30">
         <v>38869</v>
       </c>
       <c r="G16" t="s">
@@ -1383,127 +1285,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:I2"/>
-  <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10" style="31" customWidth="1"/>
-    <col min="2" max="2" width="21.83203125" style="31" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" style="31" customWidth="1"/>
-    <col min="4" max="4" width="13.5" style="31" customWidth="1"/>
-    <col min="5" max="5" width="13.5" style="1" customWidth="1"/>
-    <col min="6" max="9" width="13.5" style="31" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="F1" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="G1" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="H1" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="I1" s="34" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="28.33203125" customWidth="1"/>
-    <col min="2" max="2" width="38.83203125" customWidth="1"/>
-    <col min="3" max="3" width="60.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" style="17" customWidth="1"/>
-    <col min="5" max="5" width="29.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:S1"/>
   <sheetViews>
@@ -1536,62 +1317,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="F1" s="18" t="s">
+      <c r="D1" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="K1" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="L1" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="M1" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="N1" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="O1" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="P1" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q1" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="R1" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="S1" s="18" t="s">
-        <v>117</v>
+      <c r="G1" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="N1" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="O1" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="P1" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q1" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="R1" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="S1" s="15" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1599,7 +1380,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
@@ -1615,17 +1396,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="18" t="s">
-        <v>103</v>
+      <c r="D1" s="15" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1634,7 +1415,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -1656,55 +1437,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="B1" s="19" t="s">
+      <c r="A1" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>123</v>
+      <c r="E1" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="E2" s="3">
+        <v>98</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="1">
         <v>300</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="1">
         <v>300</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>196</v>
+      <c r="G2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1713,7 +1494,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
@@ -1730,19 +1511,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="15" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1751,7 +1532,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:O6"/>
   <sheetViews>
@@ -1761,130 +1542,130 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="21.5" style="11" customWidth="1"/>
-    <col min="3" max="3" width="15" style="11" customWidth="1"/>
-    <col min="4" max="4" width="55" style="11" customWidth="1"/>
-    <col min="5" max="5" width="48.33203125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="18.83203125" style="11" customWidth="1"/>
-    <col min="7" max="7" width="41.1640625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="15.1640625" style="11" customWidth="1"/>
-    <col min="9" max="9" width="50.5" style="11" customWidth="1"/>
-    <col min="10" max="11" width="31.5" style="11" customWidth="1"/>
-    <col min="12" max="15" width="10.83203125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="21.5" style="8" customWidth="1"/>
+    <col min="3" max="3" width="15" style="8" customWidth="1"/>
+    <col min="4" max="4" width="55" style="8" customWidth="1"/>
+    <col min="5" max="5" width="48.33203125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="41.1640625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" style="8" customWidth="1"/>
+    <col min="9" max="9" width="50.5" style="8" customWidth="1"/>
+    <col min="10" max="11" width="31.5" style="8" customWidth="1"/>
+    <col min="12" max="15" width="10.83203125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="K1" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
+      <c r="A1" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1892,7 +1673,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:J1"/>
   <sheetViews>
@@ -1912,35 +1693,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>187</v>
+      <c r="A1" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1949,7 +1730,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:G1"/>
   <sheetViews>
@@ -1963,33 +1744,33 @@
     <col min="2" max="2" width="16.83203125" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" customWidth="1"/>
     <col min="4" max="4" width="14.83203125" customWidth="1"/>
-    <col min="5" max="5" width="50.33203125" style="26" customWidth="1"/>
-    <col min="6" max="6" width="24" style="17" customWidth="1"/>
+    <col min="5" max="5" width="50.33203125" style="23" customWidth="1"/>
+    <col min="6" max="6" width="24" style="14" customWidth="1"/>
     <col min="7" max="7" width="29.6640625" customWidth="1"/>
     <col min="8" max="8" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>148</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>150</v>
+      <c r="D1" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1998,7 +1779,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -2009,65 +1790,65 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="43.83203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="7.5" style="3" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="22" style="3" customWidth="1"/>
-    <col min="7" max="7" width="54" style="3" customWidth="1"/>
-    <col min="8" max="8" width="61.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="43.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22" style="1" customWidth="1"/>
+    <col min="7" max="7" width="54" style="1" customWidth="1"/>
+    <col min="8" max="8" width="61.6640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>154</v>
+      <c r="E1" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>161</v>
+      <c r="A2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2076,63 +1857,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="12" style="31" customWidth="1"/>
-    <col min="6" max="6" width="23.1640625" customWidth="1"/>
-    <col min="7" max="7" width="20.1640625" customWidth="1"/>
-    <col min="8" max="8" width="28" customWidth="1"/>
-    <col min="9" max="9" width="28.33203125" customWidth="1"/>
-    <col min="10" max="10" width="40" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" s="35" t="s">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -2142,45 +1867,45 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5" style="3" customWidth="1"/>
-    <col min="2" max="2" width="58.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="57.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42" style="3" customWidth="1"/>
+    <col min="1" max="1" width="7.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="58.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="57.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>154</v>
+      <c r="D1" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>163</v>
+      <c r="D2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2189,7 +1914,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:G1"/>
   <sheetViews>
@@ -2208,26 +1933,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="F1" s="18" t="s">
+      <c r="D1" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="G1" s="18" t="s">
-        <v>166</v>
+      <c r="F1" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2235,7 +1960,63 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="12" style="28" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" customWidth="1"/>
+    <col min="8" max="8" width="28" customWidth="1"/>
+    <col min="9" max="9" width="28.33203125" customWidth="1"/>
+    <col min="10" max="10" width="40" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{250E6F23-B764-5243-842F-046C5535819A}">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -2245,15 +2026,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="115.83203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="115.83203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="20" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2264,7 +2045,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62A79FA-4693-DC4C-8533-78F85FC1D1D4}">
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -2281,23 +2062,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="18" t="s">
-        <v>177</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>190</v>
+      <c r="D1" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2305,7 +2086,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54F6DEFA-A517-8846-A522-4BE1FE1D8CBC}">
   <dimension ref="A1:G1"/>
   <sheetViews>
@@ -2322,26 +2103,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>176</v>
+      <c r="D1" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -2349,7 +2130,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39B0C263-3963-0B49-B113-94AC2CB14316}">
   <dimension ref="A1:E1"/>
   <sheetViews>
@@ -2359,26 +2140,26 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" style="3" customWidth="1"/>
-    <col min="2" max="3" width="17.83203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="17.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>183</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>188</v>
+      <c r="A1" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2386,7 +2167,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -2401,51 +2182,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
-        <v>167</v>
+      <c r="A1" s="16" t="s">
+        <v>141</v>
       </c>
       <c r="B1" t="s">
-        <v>168</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
-        <v>167</v>
+      <c r="A2" s="16" t="s">
+        <v>141</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="19" t="s">
-        <v>167</v>
+      <c r="A3" s="16" t="s">
+        <v>141</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="19" t="s">
-        <v>167</v>
+      <c r="A4" s="16" t="s">
+        <v>141</v>
       </c>
       <c r="B4" t="s">
-        <v>171</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="19" t="s">
-        <v>172</v>
+      <c r="A5" s="16" t="s">
+        <v>146</v>
       </c>
       <c r="B5" t="s">
-        <v>173</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
-        <v>172</v>
+      <c r="A6" s="16" t="s">
+        <v>146</v>
       </c>
       <c r="B6" t="s">
-        <v>174</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2473,43 +2254,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
-        <v>179</v>
-      </c>
-      <c r="B1" s="32" t="s">
+      <c r="A1" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="32" t="s">
-        <v>180</v>
+      <c r="F1" s="29" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>208</v>
+      <c r="B2" s="5" t="s">
+        <v>179</v>
       </c>
       <c r="C2" t="s">
-        <v>206</v>
+        <v>177</v>
       </c>
       <c r="D2" t="s">
-        <v>185</v>
+        <v>159</v>
       </c>
       <c r="E2" t="s">
         <v>37</v>
       </c>
       <c r="F2" t="s">
-        <v>207</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -2522,7 +2303,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8119FA96-6212-B14B-95A4-086E82381FB2}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -2534,23 +2315,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="36" t="s">
-        <v>178</v>
+      <c r="B1" s="33" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>209</v>
+        <v>180</v>
       </c>
       <c r="B2" t="s">
-        <v>206</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="7"/>
+      <c r="F3" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2563,7 +2344,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B9" sqref="B9:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2575,203 +2356,201 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
     </row>
     <row r="4" spans="1:6" ht="98" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="13"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="11"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="11"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="B7" s="40" t="s">
+      <c r="A7" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="11"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="11"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="11"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="40"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="11"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="11"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="11"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="11"/>
+      <c r="A13" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
+      <c r="B15" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="B16" s="9" t="s">
+      <c r="A16" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="22"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="19"/>
     </row>
     <row r="17" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="10"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="22"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="19"/>
     </row>
     <row r="18" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="21"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="22"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -2804,53 +2583,53 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="16" style="11" customWidth="1"/>
-    <col min="4" max="4" width="33.83203125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="6.5" style="11" customWidth="1"/>
-    <col min="6" max="6" width="34.83203125" style="13" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="16" style="8" customWidth="1"/>
+    <col min="4" max="4" width="33.83203125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="6.5" style="8" customWidth="1"/>
+    <col min="6" max="6" width="34.83203125" style="10" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="15" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>198</v>
+      <c r="F2" s="10" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2868,50 +2647,50 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" style="3" customWidth="1"/>
-    <col min="2" max="3" width="24.83203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="23.5" style="3" customWidth="1"/>
-    <col min="5" max="5" width="32.1640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="24.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.1640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="15" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
-        <v>192</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2937,30 +2716,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="15" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2970,177 +2749,45 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:D19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.83203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="45.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" customWidth="1"/>
+    <col min="2" max="2" width="38.83203125" customWidth="1"/>
+    <col min="3" max="3" width="60.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
-      <c r="C11" s="5"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update minimum file and regenerate
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/minimum.xlsx
+++ b/tests/integration_test_files/minimum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/github/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46366FC8-8CE9-BD46-97A4-050665DF7105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4008EF63-5AE4-2F40-8748-461FDF4AF3E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="660" windowWidth="36420" windowHeight="17380" firstSheet="12" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="820" yWindow="660" windowWidth="36420" windowHeight="17380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="166">
   <si>
     <t>name</t>
   </si>
@@ -69,9 +69,6 @@
     <t>studyRationale</t>
   </si>
   <si>
-    <t>The discontinuation rate associated with this oral dosing regimen was 58.6% in previous studies, and alternative clinical strategies have been sought to improve tolerance for the compound. To that end, development of a Transdermal Therapeutic System (TTS) has been initiated.</t>
-  </si>
-  <si>
     <t>businessTherapeuticAreas</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
     <t>study_version</t>
   </si>
   <si>
-    <t>D_APPROVE</t>
-  </si>
-  <si>
     <t>Design approval date</t>
   </si>
   <si>
@@ -174,9 +168,6 @@
     <t>therapeuticAreas</t>
   </si>
   <si>
-    <t>SPONSOR: MILD_MOD_ALZ=Mild to Moderate Alzheimer's Disease, SNOMED: 26929004=Alzheimer's disease</t>
-  </si>
-  <si>
     <t>studyDesignRationale</t>
   </si>
   <si>
@@ -522,9 +513,6 @@
     <t>Super Drug</t>
   </si>
   <si>
-    <t>This is the officlal title</t>
-  </si>
-  <si>
     <t>SPONSOR</t>
   </si>
   <si>
@@ -541,6 +529,18 @@
   </si>
   <si>
     <t>Efficacy Study</t>
+  </si>
+  <si>
+    <t>SNOMED: 26929004=Alzheimer's disease</t>
+  </si>
+  <si>
+    <t>Study design rationale in here</t>
+  </si>
+  <si>
+    <t>DESIGN_APPROVAL_DATE</t>
+  </si>
+  <si>
+    <t>MIN_STUDY</t>
   </si>
 </sst>
 </file>
@@ -1042,14 +1042,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.5" customWidth="1"/>
-    <col min="2" max="2" width="37.5" customWidth="1"/>
+    <col min="2" max="2" width="43" customWidth="1"/>
     <col min="3" max="3" width="31.33203125" customWidth="1"/>
     <col min="4" max="4" width="23.33203125" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
@@ -1062,27 +1062,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="E1" s="28"/>
       <c r="F1" s="28"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E2" s="28"/>
       <c r="F2" s="28"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E3" s="28"/>
       <c r="F3" s="28"/>
@@ -1102,54 +1102,52 @@
         <v>6</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E5" s="28"/>
       <c r="F5" s="28"/>
     </row>
-    <row r="6" spans="1:7" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="28"/>
     </row>
-    <row r="7" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E7" s="28"/>
       <c r="F7" s="28"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E8" s="28"/>
       <c r="F8" s="28"/>
     </row>
-    <row r="9" spans="1:7" ht="47" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>159</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B9" s="10"/>
       <c r="E9" s="28"/>
       <c r="F9" s="28"/>
     </row>
-    <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="10"/>
       <c r="E10" s="28"/>
@@ -1157,7 +1155,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="10"/>
       <c r="E11" s="28"/>
@@ -1165,7 +1163,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="27">
         <v>1</v>
@@ -1175,10 +1173,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="E13" s="28"/>
       <c r="F13" s="28"/>
@@ -1189,48 +1187,48 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="29" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="E15" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="F15" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="G15" s="29" t="s">
         <v>21</v>
-      </c>
-      <c r="G15" s="29" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C16" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="D16" t="s">
         <v>24</v>
       </c>
-      <c r="C16" t="s">
+      <c r="E16" t="s">
         <v>25</v>
-      </c>
-      <c r="D16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" t="s">
-        <v>27</v>
       </c>
       <c r="F16" s="30">
         <v>38869</v>
       </c>
       <c r="G16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1276,58 +1274,58 @@
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="G1" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="I1" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="15" t="s">
+      <c r="J1" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="K1" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="L1" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="M1" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="N1" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="O1" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="P1" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="Q1" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="R1" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="S1" s="15" t="s">
         <v>80</v>
-      </c>
-      <c r="Q1" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="R1" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="S1" s="15" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1355,13 +1353,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>19</v>
-      </c>
       <c r="D1" s="15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1393,42 +1391,42 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="16" t="s">
-        <v>19</v>
-      </c>
       <c r="E1" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="I1" s="16" t="s">
         <v>86</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E2" s="1">
         <v>300</v>
@@ -1437,10 +1435,10 @@
         <v>300</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1470,16 +1468,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="26" t="s">
-        <v>19</v>
-      </c>
       <c r="D1" s="26" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1512,37 +1510,37 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="E1" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="F1" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="G1" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="H1" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="I1" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="J1" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="K1" s="15" t="s">
         <v>101</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>104</v>
       </c>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
@@ -1649,34 +1647,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="F1" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="G1" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="I1" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>110</v>
-      </c>
       <c r="J1" s="15" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1710,22 +1708,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>19</v>
-      </c>
       <c r="D1" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="G1" s="12" t="s">
         <v>113</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1759,25 +1757,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>20</v>
-      </c>
       <c r="E1" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="H1" s="15" t="s">
         <v>117</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1790,7 +1788,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1808,27 +1806,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>19</v>
-      </c>
       <c r="D1" s="15" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E2" s="3"/>
     </row>
@@ -1861,22 +1859,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>19</v>
-      </c>
       <c r="D1" s="15" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1908,31 +1906,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D1" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="29" t="s">
+      <c r="H1" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="I1" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="J1" s="32" t="s">
         <v>32</v>
-      </c>
-      <c r="I1" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" s="32" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1959,7 +1957,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1990,19 +1988,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>19</v>
-      </c>
       <c r="D1" s="15" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -2031,22 +2029,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>19</v>
-      </c>
       <c r="D1" s="15" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2071,19 +2069,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -2107,50 +2105,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" t="s">
         <v>125</v>
-      </c>
-      <c r="B3" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2179,42 +2177,42 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="29" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C1" s="29" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="29" t="s">
-        <v>20</v>
-      </c>
       <c r="F1" s="29" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -2240,18 +2238,18 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2267,8 +2265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:E7"/>
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2281,10 +2279,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C1" s="36"/>
       <c r="D1" s="36"/>
@@ -2293,34 +2291,34 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
       <c r="E2" s="36"/>
       <c r="F2" s="36"/>
     </row>
-    <row r="3" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>43</v>
+        <v>162</v>
       </c>
       <c r="C3" s="36"/>
       <c r="D3" s="36"/>
       <c r="E3" s="36"/>
       <c r="F3" s="36"/>
     </row>
-    <row r="4" spans="1:6" ht="98" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>8</v>
+        <v>163</v>
       </c>
       <c r="C4" s="36"/>
       <c r="D4" s="36"/>
@@ -2329,10 +2327,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C5" s="36"/>
       <c r="D5" s="36"/>
@@ -2341,10 +2339,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C6" s="36"/>
       <c r="D6" s="36"/>
@@ -2353,10 +2351,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C7" s="36"/>
       <c r="D7" s="36"/>
@@ -2365,10 +2363,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C8" s="36"/>
       <c r="D8" s="36"/>
@@ -2377,7 +2375,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B9" s="35"/>
       <c r="C9" s="36"/>
@@ -2387,7 +2385,7 @@
     </row>
     <row r="10" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B10" s="37"/>
       <c r="C10" s="36"/>
@@ -2421,7 +2419,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B13" s="34"/>
       <c r="C13" s="34"/>
@@ -2438,10 +2436,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -2450,10 +2448,10 @@
     </row>
     <row r="16" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -2518,25 +2516,25 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="15" t="s">
-        <v>19</v>
-      </c>
       <c r="F1" s="20" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -2566,39 +2564,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>20</v>
-      </c>
       <c r="E1" s="15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2627,27 +2625,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>19</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2677,16 +2675,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>19</v>
-      </c>
       <c r="D1" s="31" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>